<commit_message>
moved instruction memory inside processor. started refactoring timer module, still not done
</commit_message>
<xml_diff>
--- a/docs/sfr_calculators.xlsx
+++ b/docs/sfr_calculators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -152,7 +152,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -166,10 +166,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -194,16 +190,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C6:I20"/>
+  <dimension ref="C6:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="16.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.67"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -242,23 +238,23 @@
         <v>22</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2" t="n">
         <f aca="false">Sheet2!$I$7</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G9" s="2" t="n">
         <f aca="false">Sheet2!$I$13</f>
-        <v>215</v>
+        <v>134</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">1000*POWER(2,F9)*G9/(D9*1000000)</f>
-        <v>22.016</v>
+        <v>21.95456</v>
       </c>
       <c r="I9" s="3" t="n">
         <f aca="false">(ABS(C9-H9)/C9)</f>
-        <v>0.000727272727272647</v>
+        <v>0.00206545454545451</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -269,18 +265,6 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -304,11 +288,11 @@
   </sheetPr>
   <dimension ref="C3:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="14.31"/>
   </cols>
@@ -324,7 +308,7 @@
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="n">
         <f aca="false">Sheet1!$D$9*1000000</f>
-        <v>10000000</v>
+        <v>50000000</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">Sheet1!$C$9/1000</f>
@@ -361,19 +345,19 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">$D$4*$C$4/D7</f>
-        <v>220000</v>
+        <v>1100000</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E7,1)&lt;256,CEILING(E7,1)&gt;0),C7,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="4" t="n">
         <f aca="false">ABS(ROUND(E7,0)-E7)/E7</f>
         <v>0</v>
       </c>
       <c r="I7" s="0" t="n">
-        <f aca="false">IF(F22=0,C22,MIN(F7:F22))</f>
-        <v>10</v>
+        <f aca="false">IF(F22=10000,C22,MIN(F7:F22))</f>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,13 +371,13 @@
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">$D$4*$C$4/D8</f>
-        <v>110000</v>
+        <v>550000</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E8,1)&lt;256,CEILING(E8,1)&gt;0),C8,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="4" t="n">
         <f aca="false">ABS(ROUND(E8,0)-E8)/E8</f>
         <v>0</v>
       </c>
@@ -409,13 +393,13 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">$D$4*$C$4/D9</f>
-        <v>55000</v>
+        <v>275000</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E9,1)&lt;256,CEILING(E9,1)&gt;0),C9,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="4" t="n">
         <f aca="false">ABS(ROUND(E9,0)-E9)/E9</f>
         <v>0</v>
       </c>
@@ -434,19 +418,19 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">$D$4*$C$4/D10</f>
-        <v>27500</v>
+        <v>137500</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E10,1)&lt;256,CEILING(E10,1)&gt;0),C10,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="4" t="n">
         <f aca="false">ABS(ROUND(E10,0)-E10)/E10</f>
         <v>0</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="true">ROUND(INDIRECT(ADDRESS(I7+7,5)),0)</f>
-        <v>215</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,13 +444,13 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">$D$4*$C$4/D11</f>
-        <v>13750</v>
+        <v>68750</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E11,1)&lt;256,CEILING(E11,1)&gt;0),C11,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="4" t="n">
         <f aca="false">ABS(ROUND(E11,0)-E11)/E11</f>
         <v>0</v>
       </c>
@@ -482,13 +466,13 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">$D$4*$C$4/D12</f>
-        <v>6875</v>
+        <v>34375</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E12,1)&lt;256,CEILING(E12,1)&gt;0),C12,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="4" t="n">
         <f aca="false">ABS(ROUND(E12,0)-E12)/E12</f>
         <v>0</v>
       </c>
@@ -507,19 +491,19 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">$D$4*$C$4/D13</f>
-        <v>3437.5</v>
+        <v>17187.5</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E13,1)&lt;256,CEILING(E13,1)&gt;0),C13,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="G13" s="4" t="n">
         <f aca="false">ABS(ROUND(E13,0)-E13)/E13</f>
-        <v>0.000145454545454545</v>
+        <v>2.90909090909091E-005</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">IF(I10&gt;255,255,IF(I10&lt;1,1,I10))</f>
-        <v>215</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,15 +517,15 @@
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">$D$4*$C$4/D14</f>
-        <v>1718.75</v>
+        <v>8593.75</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E14,1)&lt;256,CEILING(E14,1)&gt;0),C14,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="G14" s="4" t="n">
         <f aca="false">ABS(ROUND(E14,0)-E14)/E14</f>
-        <v>0.000145454545454545</v>
+        <v>2.90909090909091E-005</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,15 +539,15 @@
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">$D$4*$C$4/D15</f>
-        <v>859.375</v>
+        <v>4296.875</v>
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E15,1)&lt;256,CEILING(E15,1)&gt;0),C15,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="4" t="n">
         <f aca="false">ABS(ROUND(E15,0)-E15)/E15</f>
-        <v>0.000436363636363636</v>
+        <v>2.90909090909091E-005</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>16</v>
@@ -580,15 +564,15 @@
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">$D$4*$C$4/D16</f>
-        <v>429.6875</v>
+        <v>2148.4375</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E16,1)&lt;256,CEILING(E16,1)&gt;0),C16,10000)</f>
         <v>10000</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="4" t="n">
         <f aca="false">ABS(ROUND(E16,0)-E16)/E16</f>
-        <v>0.000727272727272727</v>
+        <v>0.000203636363636364</v>
       </c>
       <c r="I16" s="0" t="n">
         <f aca="false">IF(OR(I10&lt;1,I10&gt;255),0,1)</f>
@@ -606,15 +590,15 @@
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">$D$4*$C$4/D17</f>
-        <v>214.84375</v>
+        <v>1074.21875</v>
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E17,1)&lt;256,CEILING(E17,1)&gt;0),C17,10000)</f>
-        <v>10</v>
-      </c>
-      <c r="G17" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G17" s="4" t="n">
         <f aca="false">ABS(ROUND(E17,0)-E17)/E17</f>
-        <v>0.000727272727272727</v>
+        <v>0.000203636363636364</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,15 +612,15 @@
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">$D$4*$C$4/D18</f>
-        <v>107.421875</v>
+        <v>537.109375</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E18,1)&lt;256,CEILING(E18,1)&gt;0),C18,10000)</f>
-        <v>11</v>
-      </c>
-      <c r="G18" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G18" s="4" t="n">
         <f aca="false">ABS(ROUND(E18,0)-E18)/E18</f>
-        <v>0.00392727272727273</v>
+        <v>0.000203636363636364</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -650,15 +634,15 @@
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">$D$4*$C$4/D19</f>
-        <v>53.7109375</v>
+        <v>268.5546875</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E19,1)&lt;256,CEILING(E19,1)&gt;0),C19,10000)</f>
-        <v>12</v>
-      </c>
-      <c r="G19" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G19" s="4" t="n">
         <f aca="false">ABS(ROUND(E19,0)-E19)/E19</f>
-        <v>0.00538181818181818</v>
+        <v>0.00165818181818182</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,15 +656,15 @@
       </c>
       <c r="E20" s="0" t="n">
         <f aca="false">$D$4*$C$4/D20</f>
-        <v>26.85546875</v>
+        <v>134.27734375</v>
       </c>
       <c r="F20" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E20,1)&lt;256,CEILING(E20,1)&gt;0),C20,10000)</f>
         <v>13</v>
       </c>
-      <c r="G20" s="5" t="n">
+      <c r="G20" s="4" t="n">
         <f aca="false">ABS(ROUND(E20,0)-E20)/E20</f>
-        <v>0.00538181818181818</v>
+        <v>0.00206545454545455</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,15 +678,15 @@
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">$D$4*$C$4/D21</f>
-        <v>13.427734375</v>
+        <v>67.138671875</v>
       </c>
       <c r="F21" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E21,1)&lt;256,CEILING(E21,1)&gt;0),C21,10000)</f>
         <v>14</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" s="4" t="n">
         <f aca="false">ABS(ROUND(E21,0)-E21)/E21</f>
-        <v>0.0318545454545455</v>
+        <v>0.00206545454545455</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,15 +700,15 @@
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">$D$4*$C$4/D22</f>
-        <v>6.7138671875</v>
+        <v>33.5693359375</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E22,1)&lt;256,CEILING(E22,1)&gt;0),C22,10000)</f>
         <v>15</v>
       </c>
-      <c r="G22" s="5" t="n">
+      <c r="G22" s="4" t="n">
         <f aca="false">ABS(ROUND(E22,0)-E22)/E22</f>
-        <v>0.0426181818181818</v>
+        <v>0.0128290909090909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
timer bug fixed, blinking at correct rate
</commit_message>
<xml_diff>
--- a/docs/sfr_calculators.xlsx
+++ b/docs/sfr_calculators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -192,14 +192,14 @@
   </sheetPr>
   <dimension ref="C6:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="16.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.66"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,10 +235,11 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="n">
-        <v>22</v>
+        <v>1000</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>50</v>
+        <f aca="false">50/32</f>
+        <v>1.5625</v>
       </c>
       <c r="F9" s="2" t="n">
         <f aca="false">Sheet2!$I$7</f>
@@ -246,15 +247,15 @@
       </c>
       <c r="G9" s="2" t="n">
         <f aca="false">Sheet2!$I$13</f>
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">1000*POWER(2,F9)*G9/(D9*1000000)</f>
-        <v>21.95456</v>
+        <v>1001.39008</v>
       </c>
       <c r="I9" s="3" t="n">
         <f aca="false">(ABS(C9-H9)/C9)</f>
-        <v>0.00206545454545451</v>
+        <v>0.00139008000000001</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,11 +289,11 @@
   </sheetPr>
   <dimension ref="C3:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="14.31"/>
   </cols>
@@ -308,11 +309,11 @@
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="n">
         <f aca="false">Sheet1!$D$9*1000000</f>
-        <v>50000000</v>
+        <v>1562500</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">Sheet1!$C$9/1000</f>
-        <v>0.022</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,7 +346,7 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">$D$4*$C$4/D7</f>
-        <v>1100000</v>
+        <v>1562500</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E7,1)&lt;256,CEILING(E7,1)&gt;0),C7,10000)</f>
@@ -371,7 +372,7 @@
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">$D$4*$C$4/D8</f>
-        <v>550000</v>
+        <v>781250</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E8,1)&lt;256,CEILING(E8,1)&gt;0),C8,10000)</f>
@@ -393,7 +394,7 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">$D$4*$C$4/D9</f>
-        <v>275000</v>
+        <v>390625</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E9,1)&lt;256,CEILING(E9,1)&gt;0),C9,10000)</f>
@@ -418,7 +419,7 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">$D$4*$C$4/D10</f>
-        <v>137500</v>
+        <v>195312.5</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E10,1)&lt;256,CEILING(E10,1)&gt;0),C10,10000)</f>
@@ -426,11 +427,11 @@
       </c>
       <c r="G10" s="4" t="n">
         <f aca="false">ABS(ROUND(E10,0)-E10)/E10</f>
-        <v>0</v>
+        <v>2.56E-006</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="true">ROUND(INDIRECT(ADDRESS(I7+7,5)),0)</f>
-        <v>134</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +445,7 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">$D$4*$C$4/D11</f>
-        <v>68750</v>
+        <v>97656.25</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E11,1)&lt;256,CEILING(E11,1)&gt;0),C11,10000)</f>
@@ -452,7 +453,7 @@
       </c>
       <c r="G11" s="4" t="n">
         <f aca="false">ABS(ROUND(E11,0)-E11)/E11</f>
-        <v>0</v>
+        <v>2.56E-006</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,7 +467,7 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">$D$4*$C$4/D12</f>
-        <v>34375</v>
+        <v>48828.125</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E12,1)&lt;256,CEILING(E12,1)&gt;0),C12,10000)</f>
@@ -474,7 +475,7 @@
       </c>
       <c r="G12" s="4" t="n">
         <f aca="false">ABS(ROUND(E12,0)-E12)/E12</f>
-        <v>0</v>
+        <v>2.56E-006</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>15</v>
@@ -491,7 +492,7 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">$D$4*$C$4/D13</f>
-        <v>17187.5</v>
+        <v>24414.0625</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E13,1)&lt;256,CEILING(E13,1)&gt;0),C13,10000)</f>
@@ -499,11 +500,11 @@
       </c>
       <c r="G13" s="4" t="n">
         <f aca="false">ABS(ROUND(E13,0)-E13)/E13</f>
-        <v>2.90909090909091E-005</v>
+        <v>2.56E-006</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">IF(I10&gt;255,255,IF(I10&lt;1,1,I10))</f>
-        <v>134</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,7 +518,7 @@
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">$D$4*$C$4/D14</f>
-        <v>8593.75</v>
+        <v>12207.03125</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E14,1)&lt;256,CEILING(E14,1)&gt;0),C14,10000)</f>
@@ -525,7 +526,7 @@
       </c>
       <c r="G14" s="4" t="n">
         <f aca="false">ABS(ROUND(E14,0)-E14)/E14</f>
-        <v>2.90909090909091E-005</v>
+        <v>2.56E-006</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,7 +540,7 @@
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">$D$4*$C$4/D15</f>
-        <v>4296.875</v>
+        <v>6103.515625</v>
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E15,1)&lt;256,CEILING(E15,1)&gt;0),C15,10000)</f>
@@ -547,7 +548,7 @@
       </c>
       <c r="G15" s="4" t="n">
         <f aca="false">ABS(ROUND(E15,0)-E15)/E15</f>
-        <v>2.90909090909091E-005</v>
+        <v>7.936E-005</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>16</v>
@@ -564,7 +565,7 @@
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">$D$4*$C$4/D16</f>
-        <v>2148.4375</v>
+        <v>3051.7578125</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E16,1)&lt;256,CEILING(E16,1)&gt;0),C16,10000)</f>
@@ -572,7 +573,7 @@
       </c>
       <c r="G16" s="4" t="n">
         <f aca="false">ABS(ROUND(E16,0)-E16)/E16</f>
-        <v>0.000203636363636364</v>
+        <v>7.936E-005</v>
       </c>
       <c r="I16" s="0" t="n">
         <f aca="false">IF(OR(I10&lt;1,I10&gt;255),0,1)</f>
@@ -590,7 +591,7 @@
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">$D$4*$C$4/D17</f>
-        <v>1074.21875</v>
+        <v>1525.87890625</v>
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E17,1)&lt;256,CEILING(E17,1)&gt;0),C17,10000)</f>
@@ -598,7 +599,7 @@
       </c>
       <c r="G17" s="4" t="n">
         <f aca="false">ABS(ROUND(E17,0)-E17)/E17</f>
-        <v>0.000203636363636364</v>
+        <v>7.936E-005</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,7 +613,7 @@
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">$D$4*$C$4/D18</f>
-        <v>537.109375</v>
+        <v>762.939453125</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E18,1)&lt;256,CEILING(E18,1)&gt;0),C18,10000)</f>
@@ -620,7 +621,7 @@
       </c>
       <c r="G18" s="4" t="n">
         <f aca="false">ABS(ROUND(E18,0)-E18)/E18</f>
-        <v>0.000203636363636364</v>
+        <v>7.936E-005</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,7 +635,7 @@
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">$D$4*$C$4/D19</f>
-        <v>268.5546875</v>
+        <v>381.4697265625</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E19,1)&lt;256,CEILING(E19,1)&gt;0),C19,10000)</f>
@@ -642,7 +643,7 @@
       </c>
       <c r="G19" s="4" t="n">
         <f aca="false">ABS(ROUND(E19,0)-E19)/E19</f>
-        <v>0.00165818181818182</v>
+        <v>0.00123136</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,7 +657,7 @@
       </c>
       <c r="E20" s="0" t="n">
         <f aca="false">$D$4*$C$4/D20</f>
-        <v>134.27734375</v>
+        <v>190.73486328125</v>
       </c>
       <c r="F20" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E20,1)&lt;256,CEILING(E20,1)&gt;0),C20,10000)</f>
@@ -664,7 +665,7 @@
       </c>
       <c r="G20" s="4" t="n">
         <f aca="false">ABS(ROUND(E20,0)-E20)/E20</f>
-        <v>0.00206545454545455</v>
+        <v>0.00139008</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,7 +679,7 @@
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">$D$4*$C$4/D21</f>
-        <v>67.138671875</v>
+        <v>95.367431640625</v>
       </c>
       <c r="F21" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E21,1)&lt;256,CEILING(E21,1)&gt;0),C21,10000)</f>
@@ -686,7 +687,7 @@
       </c>
       <c r="G21" s="4" t="n">
         <f aca="false">ABS(ROUND(E21,0)-E21)/E21</f>
-        <v>0.00206545454545455</v>
+        <v>0.0038528</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,7 +701,7 @@
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">$D$4*$C$4/D22</f>
-        <v>33.5693359375</v>
+        <v>47.6837158203125</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E22,1)&lt;256,CEILING(E22,1)&gt;0),C22,10000)</f>
@@ -708,7 +709,7 @@
       </c>
       <c r="G22" s="4" t="n">
         <f aca="false">ABS(ROUND(E22,0)-E22)/E22</f>
-        <v>0.0128290909090909</v>
+        <v>0.00663296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in delay_ms function. still working on uart in hw.
</commit_message>
<xml_diff>
--- a/docs/sfr_calculators.xlsx
+++ b/docs/sfr_calculators.xlsx
@@ -190,13 +190,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C6:I12"/>
+  <dimension ref="B6:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="16.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.66"/>
@@ -235,7 +235,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="n">
-        <v>1000</v>
+        <v>0.00434</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">50/32</f>
@@ -243,22 +243,26 @@
       </c>
       <c r="F9" s="2" t="n">
         <f aca="false">Sheet2!$I$7</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
         <f aca="false">Sheet2!$I$13</f>
-        <v>191</v>
+        <v>7</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">1000*POWER(2,F9)*G9/(D9*1000000)</f>
-        <v>1001.39008</v>
+        <v>0.00448</v>
       </c>
       <c r="I9" s="3" t="n">
         <f aca="false">(ABS(C9-H9)/C9)</f>
-        <v>0.00139008000000001</v>
+        <v>0.0322580645161289</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <f aca="false">1000*0.5/115200</f>
+        <v>0.00434027777777778</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -293,7 +297,7 @@
       <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="14.31"/>
   </cols>
@@ -313,7 +317,7 @@
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">Sheet1!$C$9/1000</f>
-        <v>1</v>
+        <v>4.34E-006</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -346,19 +350,19 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">$D$4*$C$4/D7</f>
-        <v>1562500</v>
+        <v>6.78125</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E7,1)&lt;256,CEILING(E7,1)&gt;0),C7,10000)</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G7" s="4" t="n">
         <f aca="false">ABS(ROUND(E7,0)-E7)/E7</f>
-        <v>0</v>
+        <v>0.032258064516129</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">IF(F22=10000,C22,MIN(F7:F22))</f>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,15 +376,15 @@
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">$D$4*$C$4/D8</f>
-        <v>781250</v>
+        <v>3.390625</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E8,1)&lt;256,CEILING(E8,1)&gt;0),C8,10000)</f>
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4" t="n">
         <f aca="false">ABS(ROUND(E8,0)-E8)/E8</f>
-        <v>0</v>
+        <v>0.115207373271889</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,15 +398,15 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">$D$4*$C$4/D9</f>
-        <v>390625</v>
+        <v>1.6953125</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E9,1)&lt;256,CEILING(E9,1)&gt;0),C9,10000)</f>
-        <v>10000</v>
+        <v>2</v>
       </c>
       <c r="G9" s="4" t="n">
         <f aca="false">ABS(ROUND(E9,0)-E9)/E9</f>
-        <v>0</v>
+        <v>0.179723502304147</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>11</v>
@@ -419,19 +423,19 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">$D$4*$C$4/D10</f>
-        <v>195312.5</v>
+        <v>0.84765625</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E10,1)&lt;256,CEILING(E10,1)&gt;0),C10,10000)</f>
-        <v>10000</v>
+        <v>3</v>
       </c>
       <c r="G10" s="4" t="n">
         <f aca="false">ABS(ROUND(E10,0)-E10)/E10</f>
-        <v>2.56E-006</v>
+        <v>0.179723502304147</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="true">ROUND(INDIRECT(ADDRESS(I7+7,5)),0)</f>
-        <v>191</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,15 +449,15 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">$D$4*$C$4/D11</f>
-        <v>97656.25</v>
+        <v>0.423828125</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E11,1)&lt;256,CEILING(E11,1)&gt;0),C11,10000)</f>
-        <v>10000</v>
+        <v>4</v>
       </c>
       <c r="G11" s="4" t="n">
         <f aca="false">ABS(ROUND(E11,0)-E11)/E11</f>
-        <v>2.56E-006</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,15 +471,15 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">$D$4*$C$4/D12</f>
-        <v>48828.125</v>
+        <v>0.2119140625</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E12,1)&lt;256,CEILING(E12,1)&gt;0),C12,10000)</f>
-        <v>10000</v>
+        <v>5</v>
       </c>
       <c r="G12" s="4" t="n">
         <f aca="false">ABS(ROUND(E12,0)-E12)/E12</f>
-        <v>2.56E-006</v>
+        <v>1</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>15</v>
@@ -492,19 +496,19 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">$D$4*$C$4/D13</f>
-        <v>24414.0625</v>
+        <v>0.10595703125</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E13,1)&lt;256,CEILING(E13,1)&gt;0),C13,10000)</f>
-        <v>10000</v>
+        <v>6</v>
       </c>
       <c r="G13" s="4" t="n">
         <f aca="false">ABS(ROUND(E13,0)-E13)/E13</f>
-        <v>2.56E-006</v>
+        <v>1</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">IF(I10&gt;255,255,IF(I10&lt;1,1,I10))</f>
-        <v>191</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -518,15 +522,15 @@
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">$D$4*$C$4/D14</f>
-        <v>12207.03125</v>
+        <v>0.052978515625</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E14,1)&lt;256,CEILING(E14,1)&gt;0),C14,10000)</f>
-        <v>10000</v>
+        <v>7</v>
       </c>
       <c r="G14" s="4" t="n">
         <f aca="false">ABS(ROUND(E14,0)-E14)/E14</f>
-        <v>2.56E-006</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,15 +544,15 @@
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">$D$4*$C$4/D15</f>
-        <v>6103.515625</v>
+        <v>0.0264892578125</v>
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E15,1)&lt;256,CEILING(E15,1)&gt;0),C15,10000)</f>
-        <v>10000</v>
+        <v>8</v>
       </c>
       <c r="G15" s="4" t="n">
         <f aca="false">ABS(ROUND(E15,0)-E15)/E15</f>
-        <v>7.936E-005</v>
+        <v>1</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>16</v>
@@ -565,15 +569,15 @@
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">$D$4*$C$4/D16</f>
-        <v>3051.7578125</v>
+        <v>0.01324462890625</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E16,1)&lt;256,CEILING(E16,1)&gt;0),C16,10000)</f>
-        <v>10000</v>
+        <v>9</v>
       </c>
       <c r="G16" s="4" t="n">
         <f aca="false">ABS(ROUND(E16,0)-E16)/E16</f>
-        <v>7.936E-005</v>
+        <v>1</v>
       </c>
       <c r="I16" s="0" t="n">
         <f aca="false">IF(OR(I10&lt;1,I10&gt;255),0,1)</f>
@@ -591,15 +595,15 @@
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">$D$4*$C$4/D17</f>
-        <v>1525.87890625</v>
+        <v>0.006622314453125</v>
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E17,1)&lt;256,CEILING(E17,1)&gt;0),C17,10000)</f>
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="G17" s="4" t="n">
         <f aca="false">ABS(ROUND(E17,0)-E17)/E17</f>
-        <v>7.936E-005</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,15 +617,15 @@
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">$D$4*$C$4/D18</f>
-        <v>762.939453125</v>
+        <v>0.0033111572265625</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E18,1)&lt;256,CEILING(E18,1)&gt;0),C18,10000)</f>
-        <v>10000</v>
+        <v>11</v>
       </c>
       <c r="G18" s="4" t="n">
         <f aca="false">ABS(ROUND(E18,0)-E18)/E18</f>
-        <v>7.936E-005</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,15 +639,15 @@
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">$D$4*$C$4/D19</f>
-        <v>381.4697265625</v>
+        <v>0.00165557861328125</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E19,1)&lt;256,CEILING(E19,1)&gt;0),C19,10000)</f>
-        <v>10000</v>
+        <v>12</v>
       </c>
       <c r="G19" s="4" t="n">
         <f aca="false">ABS(ROUND(E19,0)-E19)/E19</f>
-        <v>0.00123136</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,7 +661,7 @@
       </c>
       <c r="E20" s="0" t="n">
         <f aca="false">$D$4*$C$4/D20</f>
-        <v>190.73486328125</v>
+        <v>0.000827789306640625</v>
       </c>
       <c r="F20" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E20,1)&lt;256,CEILING(E20,1)&gt;0),C20,10000)</f>
@@ -665,7 +669,7 @@
       </c>
       <c r="G20" s="4" t="n">
         <f aca="false">ABS(ROUND(E20,0)-E20)/E20</f>
-        <v>0.00139008</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,7 +683,7 @@
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">$D$4*$C$4/D21</f>
-        <v>95.367431640625</v>
+        <v>0.000413894653320313</v>
       </c>
       <c r="F21" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E21,1)&lt;256,CEILING(E21,1)&gt;0),C21,10000)</f>
@@ -687,7 +691,7 @@
       </c>
       <c r="G21" s="4" t="n">
         <f aca="false">ABS(ROUND(E21,0)-E21)/E21</f>
-        <v>0.0038528</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,7 +705,7 @@
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">$D$4*$C$4/D22</f>
-        <v>47.6837158203125</v>
+        <v>0.000206947326660156</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E22,1)&lt;256,CEILING(E22,1)&gt;0),C22,10000)</f>
@@ -709,7 +713,7 @@
       </c>
       <c r="G22" s="4" t="n">
         <f aca="false">ABS(ROUND(E22,0)-E22)/E22</f>
-        <v>0.00663296</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving latest uart stuff
</commit_message>
<xml_diff>
--- a/docs/sfr_calculators.xlsx
+++ b/docs/sfr_calculators.xlsx
@@ -90,7 +90,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -193,16 +192,18 @@
   <dimension ref="B6:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="16.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="11" style="0" width="8.72"/>
   </cols>
   <sheetData>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -213,7 +214,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
         <v>1</v>
       </c>
@@ -235,7 +236,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="n">
-        <v>0.00434</v>
+        <v>500</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">50/32</f>
@@ -243,19 +244,19 @@
       </c>
       <c r="F9" s="2" t="n">
         <f aca="false">Sheet2!$I$7</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G9" s="2" t="n">
         <f aca="false">Sheet2!$I$13</f>
-        <v>7</v>
+        <v>191</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">1000*POWER(2,F9)*G9/(D9*1000000)</f>
-        <v>0.00448</v>
+        <v>500.69504</v>
       </c>
       <c r="I9" s="3" t="n">
         <f aca="false">(ABS(C9-H9)/C9)</f>
-        <v>0.0322580645161289</v>
+        <v>0.00139008000000001</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,12 +298,14 @@
       <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="8" style="0" width="8.72"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
@@ -310,17 +313,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="n">
         <f aca="false">Sheet1!$D$9*1000000</f>
         <v>1562500</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">Sheet1!$C$9/1000</f>
-        <v>4.34E-006</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
         <v>9</v>
       </c>
@@ -350,22 +353,22 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">$D$4*$C$4/D7</f>
-        <v>6.78125</v>
+        <v>781250</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E7,1)&lt;256,CEILING(E7,1)&gt;0),C7,10000)</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="G7" s="4" t="n">
         <f aca="false">ABS(ROUND(E7,0)-E7)/E7</f>
-        <v>0.032258064516129</v>
+        <v>0</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">IF(F22=10000,C22,MIN(F7:F22))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="n">
         <f aca="false">C7+1</f>
         <v>1</v>
@@ -376,15 +379,15 @@
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">$D$4*$C$4/D8</f>
-        <v>3.390625</v>
+        <v>390625</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E8,1)&lt;256,CEILING(E8,1)&gt;0),C8,10000)</f>
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="G8" s="4" t="n">
         <f aca="false">ABS(ROUND(E8,0)-E8)/E8</f>
-        <v>0.115207373271889</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -398,15 +401,15 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">$D$4*$C$4/D9</f>
-        <v>1.6953125</v>
+        <v>195312.5</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E9,1)&lt;256,CEILING(E9,1)&gt;0),C9,10000)</f>
-        <v>2</v>
+        <v>10000</v>
       </c>
       <c r="G9" s="4" t="n">
         <f aca="false">ABS(ROUND(E9,0)-E9)/E9</f>
-        <v>0.179723502304147</v>
+        <v>2.56E-006</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>11</v>
@@ -423,19 +426,19 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">$D$4*$C$4/D10</f>
-        <v>0.84765625</v>
+        <v>97656.25</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E10,1)&lt;256,CEILING(E10,1)&gt;0),C10,10000)</f>
-        <v>3</v>
+        <v>10000</v>
       </c>
       <c r="G10" s="4" t="n">
         <f aca="false">ABS(ROUND(E10,0)-E10)/E10</f>
-        <v>0.179723502304147</v>
+        <v>2.56E-006</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="true">ROUND(INDIRECT(ADDRESS(I7+7,5)),0)</f>
-        <v>7</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,15 +452,15 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">$D$4*$C$4/D11</f>
-        <v>0.423828125</v>
+        <v>48828.125</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E11,1)&lt;256,CEILING(E11,1)&gt;0),C11,10000)</f>
-        <v>4</v>
+        <v>10000</v>
       </c>
       <c r="G11" s="4" t="n">
         <f aca="false">ABS(ROUND(E11,0)-E11)/E11</f>
-        <v>1</v>
+        <v>2.56E-006</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,15 +474,15 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">$D$4*$C$4/D12</f>
-        <v>0.2119140625</v>
+        <v>24414.0625</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E12,1)&lt;256,CEILING(E12,1)&gt;0),C12,10000)</f>
-        <v>5</v>
+        <v>10000</v>
       </c>
       <c r="G12" s="4" t="n">
         <f aca="false">ABS(ROUND(E12,0)-E12)/E12</f>
-        <v>1</v>
+        <v>2.56E-006</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>15</v>
@@ -496,19 +499,19 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">$D$4*$C$4/D13</f>
-        <v>0.10595703125</v>
+        <v>12207.03125</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E13,1)&lt;256,CEILING(E13,1)&gt;0),C13,10000)</f>
-        <v>6</v>
+        <v>10000</v>
       </c>
       <c r="G13" s="4" t="n">
         <f aca="false">ABS(ROUND(E13,0)-E13)/E13</f>
-        <v>1</v>
+        <v>2.56E-006</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">IF(I10&gt;255,255,IF(I10&lt;1,1,I10))</f>
-        <v>7</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -522,15 +525,15 @@
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">$D$4*$C$4/D14</f>
-        <v>0.052978515625</v>
+        <v>6103.515625</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E14,1)&lt;256,CEILING(E14,1)&gt;0),C14,10000)</f>
-        <v>7</v>
+        <v>10000</v>
       </c>
       <c r="G14" s="4" t="n">
         <f aca="false">ABS(ROUND(E14,0)-E14)/E14</f>
-        <v>1</v>
+        <v>7.936E-005</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,15 +547,15 @@
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">$D$4*$C$4/D15</f>
-        <v>0.0264892578125</v>
+        <v>3051.7578125</v>
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E15,1)&lt;256,CEILING(E15,1)&gt;0),C15,10000)</f>
-        <v>8</v>
+        <v>10000</v>
       </c>
       <c r="G15" s="4" t="n">
         <f aca="false">ABS(ROUND(E15,0)-E15)/E15</f>
-        <v>1</v>
+        <v>7.936E-005</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>16</v>
@@ -569,15 +572,15 @@
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">$D$4*$C$4/D16</f>
-        <v>0.01324462890625</v>
+        <v>1525.87890625</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E16,1)&lt;256,CEILING(E16,1)&gt;0),C16,10000)</f>
-        <v>9</v>
+        <v>10000</v>
       </c>
       <c r="G16" s="4" t="n">
         <f aca="false">ABS(ROUND(E16,0)-E16)/E16</f>
-        <v>1</v>
+        <v>7.936E-005</v>
       </c>
       <c r="I16" s="0" t="n">
         <f aca="false">IF(OR(I10&lt;1,I10&gt;255),0,1)</f>
@@ -595,15 +598,15 @@
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">$D$4*$C$4/D17</f>
-        <v>0.006622314453125</v>
+        <v>762.939453125</v>
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E17,1)&lt;256,CEILING(E17,1)&gt;0),C17,10000)</f>
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="G17" s="4" t="n">
         <f aca="false">ABS(ROUND(E17,0)-E17)/E17</f>
-        <v>1</v>
+        <v>7.936E-005</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,15 +620,15 @@
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">$D$4*$C$4/D18</f>
-        <v>0.0033111572265625</v>
+        <v>381.4697265625</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E18,1)&lt;256,CEILING(E18,1)&gt;0),C18,10000)</f>
-        <v>11</v>
+        <v>10000</v>
       </c>
       <c r="G18" s="4" t="n">
         <f aca="false">ABS(ROUND(E18,0)-E18)/E18</f>
-        <v>1</v>
+        <v>0.00123136</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,7 +642,7 @@
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">$D$4*$C$4/D19</f>
-        <v>0.00165557861328125</v>
+        <v>190.73486328125</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E19,1)&lt;256,CEILING(E19,1)&gt;0),C19,10000)</f>
@@ -647,7 +650,7 @@
       </c>
       <c r="G19" s="4" t="n">
         <f aca="false">ABS(ROUND(E19,0)-E19)/E19</f>
-        <v>1</v>
+        <v>0.00139008</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +664,7 @@
       </c>
       <c r="E20" s="0" t="n">
         <f aca="false">$D$4*$C$4/D20</f>
-        <v>0.000827789306640625</v>
+        <v>95.367431640625</v>
       </c>
       <c r="F20" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E20,1)&lt;256,CEILING(E20,1)&gt;0),C20,10000)</f>
@@ -669,7 +672,7 @@
       </c>
       <c r="G20" s="4" t="n">
         <f aca="false">ABS(ROUND(E20,0)-E20)/E20</f>
-        <v>1</v>
+        <v>0.0038528</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -683,7 +686,7 @@
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">$D$4*$C$4/D21</f>
-        <v>0.000413894653320313</v>
+        <v>47.6837158203125</v>
       </c>
       <c r="F21" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E21,1)&lt;256,CEILING(E21,1)&gt;0),C21,10000)</f>
@@ -691,7 +694,7 @@
       </c>
       <c r="G21" s="4" t="n">
         <f aca="false">ABS(ROUND(E21,0)-E21)/E21</f>
-        <v>1</v>
+        <v>0.00663296</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,7 +708,7 @@
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">$D$4*$C$4/D22</f>
-        <v>0.000206947326660156</v>
+        <v>23.8418579101562</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">IF(AND(FLOOR(E22,1)&lt;256,CEILING(E22,1)&gt;0),C22,10000)</f>
@@ -713,7 +716,7 @@
       </c>
       <c r="G22" s="4" t="n">
         <f aca="false">ABS(ROUND(E22,0)-E22)/E22</f>
-        <v>1</v>
+        <v>0.00663296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>